<commit_message>
Reestructuración post pruebas libreria excel
</commit_message>
<xml_diff>
--- a/TeacherData.xlsx
+++ b/TeacherData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Id</t>
   </si>
@@ -28,19 +28,52 @@
     <t>Profile Route</t>
   </si>
   <si>
+    <t>60428291dd67af3fd4fe2aa9</t>
+  </si>
+  <si>
+    <t>Sebastian Antonio</t>
+  </si>
+  <si>
+    <t>Que te importaaaaaa</t>
+  </si>
+  <si>
+    <t>ejemplo@email.com</t>
+  </si>
+  <si>
+    <t>no_data</t>
+  </si>
+  <si>
+    <t>604507188a1ae91bb88ccb31</t>
+  </si>
+  <si>
+    <t>Que te importa</t>
+  </si>
+  <si>
+    <t>60483ffb2b665b41accbd942</t>
+  </si>
+  <si>
+    <t>correo@email.com</t>
+  </si>
+  <si>
+    <t>60490d8bfebb4221ac35df72</t>
+  </si>
+  <si>
+    <t>Cortés Pérez</t>
+  </si>
+  <si>
+    <t>correo3@email.com</t>
+  </si>
+  <si>
     <t>604924af5f9b641c8c810407</t>
   </si>
   <si>
-    <t>Sebastian Antonio</t>
-  </si>
-  <si>
-    <t>Cortés Pérez</t>
-  </si>
-  <si>
     <t>sebastiancortes.777@protonmail.com</t>
   </si>
   <si>
-    <t>no_data</t>
+    <t>60498975a451850f446c175a</t>
+  </si>
+  <si>
+    <t>sebastiancortes.2202@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -80,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -120,6 +153,91 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>